<commit_message>
all admin and some user functionalities
</commit_message>
<xml_diff>
--- a/toBeUploaded.xlsx
+++ b/toBeUploaded.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>companyName</t>
   </si>
@@ -36,18 +36,12 @@
     <t>dateOfPrice</t>
   </si>
   <si>
-    <t>abcd1111</t>
-  </si>
-  <si>
     <t>bse</t>
   </si>
   <si>
     <t>2020-12-16T09:13:00.0000000</t>
   </si>
   <si>
-    <t>abcd1</t>
-  </si>
-  <si>
     <t>nse</t>
   </si>
   <si>
@@ -55,6 +49,27 @@
   </si>
   <si>
     <t>2020-12-18T09:00:00.0000000</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>finance</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>abcd2222</t>
+  </si>
+  <si>
+    <t>abcd2</t>
+  </si>
+  <si>
+    <t>energy</t>
   </si>
 </sst>
 </file>
@@ -372,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,7 +402,7 @@
     <col min="5" max="5" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,56 +418,88 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>55</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
       </c>
       <c r="D3">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
       <c r="D4">
         <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>